<commit_message>
Updated routekaart status for UMC Utrecht. version 20a.
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_cure.xlsx
+++ b/src/data/routekaart_status_cure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\060.37543 NIVZ\Data\Zorginstellingen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCE5AFB-67F9-4456-9B3E-642D774874BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936A5E12-2FFF-4104-9263-BA544C7FFF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8310" yWindow="3300" windowWidth="15960" windowHeight="11835" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="1860" yWindow="870" windowWidth="18910" windowHeight="18960" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -573,17 +573,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="41.7265625" customWidth="1"/>
+    <col min="2" max="2" width="33.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
@@ -591,7 +589,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -599,7 +597,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -607,7 +605,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -615,7 +613,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -623,7 +621,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -631,7 +629,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -639,7 +637,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -647,7 +645,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -655,7 +653,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -663,7 +661,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -671,7 +669,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -679,7 +677,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -687,7 +685,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -695,7 +693,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -703,7 +701,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -711,7 +709,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -719,7 +717,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -727,7 +725,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -735,7 +733,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -743,7 +741,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -751,7 +749,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -759,7 +757,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -767,7 +765,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -775,7 +773,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -783,7 +781,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -791,7 +789,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -799,7 +797,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -807,7 +805,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -815,7 +813,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -823,7 +821,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -831,7 +829,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -839,7 +837,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -847,7 +845,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -855,7 +853,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -863,7 +861,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -871,7 +869,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -879,7 +877,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -887,7 +885,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -895,7 +893,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -903,7 +901,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -911,7 +909,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -919,7 +917,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -927,7 +925,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -935,7 +933,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -943,7 +941,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>34</v>
       </c>
@@ -951,7 +949,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -959,7 +957,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -967,15 +965,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>27</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -983,7 +981,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -991,7 +989,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -999,7 +997,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1007,7 +1005,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>33</v>
       </c>
@@ -1015,7 +1013,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1023,7 +1021,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Updated data for cure (v29)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_cure.xlsx
+++ b/src/data/routekaart_status_cure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781904A6-267C-475A-88D1-20DADD7A6B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A854C711-8E39-4BB3-AD2C-71AF59C49EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13450" yWindow="1090" windowWidth="19020" windowHeight="19120" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="2370" yWindow="1050" windowWidth="25065" windowHeight="14340" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="70">
   <si>
     <t>Amsterdam UMC</t>
   </si>
@@ -233,6 +233,12 @@
   </si>
   <si>
     <t>CuraMare</t>
+  </si>
+  <si>
+    <t>Antoni van Leeuwenhoek</t>
+  </si>
+  <si>
+    <t>Admiraal De Ruyter Ziekenhuis</t>
   </si>
 </sst>
 </file>
@@ -593,17 +599,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.7265625" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
@@ -611,521 +619,537 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>41</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>67</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>60</v>
       </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>42</v>
       </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>37</v>
       </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>8</v>
       </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>44</v>
       </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>9</v>
       </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>45</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B55" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>34</v>
-      </c>
-      <c r="B41" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>7</v>
-      </c>
-      <c r="B48" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>17</v>
-      </c>
-      <c r="B53" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>64</v>
       </c>
-      <c r="B55" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="B57" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>56</v>
       </c>
-      <c r="B56" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
+      <c r="B58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>22</v>
-      </c>
-      <c r="B57" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>21</v>
       </c>
-      <c r="B62" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>36</v>
       </c>
-      <c r="B63" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+      <c r="B65" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>65</v>
       </c>
-      <c r="B64" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+      <c r="B66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>59</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B67" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B57">
-    <sortCondition ref="A2:A57"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B58">
+    <sortCondition ref="A2:A58"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated data for cure (v30)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_cure.xlsx
+++ b/src/data/routekaart_status_cure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A854C711-8E39-4BB3-AD2C-71AF59C49EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BBFE41-E10B-42E6-BC4C-4C9D6A919220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="1050" windowWidth="25065" windowHeight="14340" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="14660" yWindow="2650" windowWidth="22880" windowHeight="14900" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="71">
   <si>
     <t>Amsterdam UMC</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>Admiraal De Ruyter Ziekenhuis</t>
+  </si>
+  <si>
+    <t>Meander Medisch Centrum</t>
   </si>
 </sst>
 </file>
@@ -599,19 +602,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.7109375" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="41.7265625" customWidth="1"/>
+    <col min="2" max="2" width="33.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
@@ -619,7 +620,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -627,7 +628,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -635,7 +636,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -643,7 +644,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -651,7 +652,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -659,7 +660,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -667,7 +668,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -675,7 +676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -683,7 +684,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -691,7 +692,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -699,7 +700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -707,7 +708,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -715,7 +716,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -723,7 +724,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -731,7 +732,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -739,7 +740,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -747,7 +748,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -755,7 +756,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -763,7 +764,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -771,7 +772,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -779,7 +780,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -787,7 +788,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -795,7 +796,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -803,7 +804,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -811,7 +812,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -819,7 +820,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -827,7 +828,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -835,7 +836,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -843,313 +844,321 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>46</v>
       </c>
-      <c r="B30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>12</v>
       </c>
-      <c r="B31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>38</v>
       </c>
-      <c r="B33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>11</v>
       </c>
-      <c r="B34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>39</v>
       </c>
-      <c r="B35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>15</v>
       </c>
-      <c r="B36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>33</v>
       </c>
-      <c r="B37" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>47</v>
       </c>
-      <c r="B38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>61</v>
       </c>
-      <c r="B39" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>48</v>
-      </c>
-      <c r="B40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>13</v>
       </c>
       <c r="B41" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>62</v>
       </c>
-      <c r="B42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>34</v>
       </c>
-      <c r="B43" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>63</v>
       </c>
-      <c r="B44" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>49</v>
       </c>
-      <c r="B45" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>26</v>
       </c>
-      <c r="B46" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>14</v>
       </c>
-      <c r="B47" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>50</v>
       </c>
-      <c r="B48" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>19</v>
       </c>
-      <c r="B49" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>7</v>
       </c>
-      <c r="B50" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="B51" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>52</v>
       </c>
-      <c r="B52" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>53</v>
       </c>
-      <c r="B53" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="B54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>54</v>
       </c>
-      <c r="B54" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="B55" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>17</v>
       </c>
-      <c r="B55" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="B56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>55</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>64</v>
       </c>
-      <c r="B57" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="B58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>56</v>
       </c>
-      <c r="B58" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>22</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>57</v>
       </c>
-      <c r="B60" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="B61" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>58</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>35</v>
       </c>
-      <c r="B62" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="B63" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>20</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>21</v>
       </c>
-      <c r="B64" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="B65" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>36</v>
       </c>
-      <c r="B65" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="B66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>65</v>
       </c>
-      <c r="B66" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="B67" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>59</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B58">
-    <sortCondition ref="A2:A58"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B59">
+    <sortCondition ref="A2:A59"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated data for cure (v33)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_cure.xlsx
+++ b/src/data/routekaart_status_cure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BBFE41-E10B-42E6-BC4C-4C9D6A919220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105C6609-F690-464E-A70E-7C9D8332B617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14660" yWindow="2650" windowWidth="22880" windowHeight="14900" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="17740" yWindow="2150" windowWidth="18170" windowHeight="14090" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -604,7 +604,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -937,7 +939,7 @@
         <v>48</v>
       </c>
       <c r="B41" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated cure data (v35)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_cure.xlsx
+++ b/src/data/routekaart_status_cure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105C6609-F690-464E-A70E-7C9D8332B617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452BA3C6-0BD0-49A9-A1A1-532729E5BAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17740" yWindow="2150" windowWidth="18170" windowHeight="14090" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="7850" yWindow="720" windowWidth="24570" windowHeight="14690" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -604,9 +604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1107,7 +1105,7 @@
         <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated cure data (v36)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_cure.xlsx
+++ b/src/data/routekaart_status_cure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452BA3C6-0BD0-49A9-A1A1-532729E5BAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68E634A-3012-466C-B848-9A921F0CA461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7850" yWindow="720" windowWidth="24570" windowHeight="14690" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="3910" yWindow="970" windowWidth="24780" windowHeight="16070" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -625,7 +625,7 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated cure data (v37)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_cure.xlsx
+++ b/src/data/routekaart_status_cure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68E634A-3012-466C-B848-9A921F0CA461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D53B14-7C90-4915-A8FB-CAA8ACF8121D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3910" yWindow="970" windowWidth="24780" windowHeight="16070" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="330" yWindow="2280" windowWidth="20040" windowHeight="18180" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="76">
   <si>
     <t>Amsterdam UMC</t>
   </si>
@@ -242,6 +242,21 @@
   </si>
   <si>
     <t>Meander Medisch Centrum</t>
+  </si>
+  <si>
+    <t>Dialysecentrum Ravenstein</t>
+  </si>
+  <si>
+    <t>Dianet</t>
+  </si>
+  <si>
+    <t>LangeLand Ziekenhuis</t>
+  </si>
+  <si>
+    <t>Revalidatiecentrum Roessingh</t>
+  </si>
+  <si>
+    <t>Rivas Zorggroep</t>
   </si>
 </sst>
 </file>
@@ -602,7 +617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -726,23 +741,23 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
@@ -750,7 +765,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
@@ -758,7 +773,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
@@ -766,7 +781,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
         <v>24</v>
@@ -774,7 +789,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
@@ -782,7 +797,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
         <v>24</v>
@@ -790,7 +805,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -798,7 +813,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
@@ -806,7 +821,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
@@ -814,7 +829,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
@@ -822,7 +837,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -830,7 +845,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
@@ -838,7 +853,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
@@ -846,7 +861,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
         <v>24</v>
@@ -854,7 +869,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
@@ -862,7 +877,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
         <v>24</v>
@@ -870,7 +885,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
         <v>24</v>
@@ -878,7 +893,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
         <v>24</v>
@@ -886,7 +901,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B35" t="s">
         <v>24</v>
@@ -894,7 +909,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
         <v>24</v>
@@ -902,7 +917,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
         <v>24</v>
@@ -910,7 +925,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B38" t="s">
         <v>24</v>
@@ -918,7 +933,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
         <v>24</v>
@@ -926,7 +941,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
         <v>24</v>
@@ -934,7 +949,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B41" t="s">
         <v>24</v>
@@ -942,15 +957,15 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
         <v>24</v>
@@ -958,7 +973,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
         <v>24</v>
@@ -966,15 +981,15 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="B46" t="s">
         <v>24</v>
@@ -982,15 +997,15 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="B48" t="s">
         <v>24</v>
@@ -998,7 +1013,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B49" t="s">
         <v>24</v>
@@ -1006,7 +1021,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="B50" t="s">
         <v>24</v>
@@ -1014,7 +1029,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
         <v>24</v>
@@ -1022,7 +1037,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="B52" t="s">
         <v>24</v>
@@ -1030,7 +1045,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="B53" t="s">
         <v>24</v>
@@ -1038,7 +1053,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B54" t="s">
         <v>24</v>
@@ -1046,7 +1061,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="B55" t="s">
         <v>24</v>
@@ -1054,7 +1069,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B56" t="s">
         <v>24</v>
@@ -1062,15 +1077,15 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B57" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B58" t="s">
         <v>24</v>
@@ -1078,7 +1093,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B59" t="s">
         <v>24</v>
@@ -1086,15 +1101,15 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B60" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B61" t="s">
         <v>24</v>
@@ -1102,15 +1117,15 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B63" t="s">
         <v>24</v>
@@ -1118,23 +1133,23 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B64" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B65" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B66" t="s">
         <v>24</v>
@@ -1142,7 +1157,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B67" t="s">
         <v>24</v>
@@ -1150,9 +1165,49 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
+        <v>35</v>
+      </c>
+      <c r="B68" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>65</v>
+      </c>
+      <c r="B72" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>59</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B73" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated cure data (v38)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_cure.xlsx
+++ b/src/data/routekaart_status_cure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D53B14-7C90-4915-A8FB-CAA8ACF8121D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36880CA4-52DB-4BD0-9936-43894316A7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="2280" windowWidth="20040" windowHeight="18180" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="1940" yWindow="4570" windowWidth="23610" windowHeight="16360" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="73">
   <si>
     <t>Amsterdam UMC</t>
   </si>
@@ -244,16 +244,7 @@
     <t>Meander Medisch Centrum</t>
   </si>
   <si>
-    <t>Dialysecentrum Ravenstein</t>
-  </si>
-  <si>
-    <t>Dianet</t>
-  </si>
-  <si>
     <t>LangeLand Ziekenhuis</t>
-  </si>
-  <si>
-    <t>Revalidatiecentrum Roessingh</t>
   </si>
   <si>
     <t>Rivas Zorggroep</t>
@@ -617,9 +608,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -664,7 +657,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -728,7 +721,7 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -741,23 +734,23 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
         <v>24</v>
@@ -765,7 +758,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
@@ -773,7 +766,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
@@ -781,7 +774,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
         <v>24</v>
@@ -789,7 +782,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
@@ -797,7 +790,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
         <v>24</v>
@@ -805,7 +798,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -813,7 +806,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
@@ -821,7 +814,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
@@ -829,7 +822,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
@@ -837,7 +830,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -845,7 +838,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
@@ -853,7 +846,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
@@ -861,7 +854,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
         <v>24</v>
@@ -869,7 +862,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
@@ -877,7 +870,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
         <v>24</v>
@@ -885,7 +878,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
         <v>24</v>
@@ -893,7 +886,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>24</v>
@@ -901,7 +894,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
         <v>24</v>
@@ -909,7 +902,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
         <v>24</v>
@@ -917,7 +910,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
         <v>24</v>
@@ -925,7 +918,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
         <v>24</v>
@@ -933,7 +926,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
         <v>24</v>
@@ -941,7 +934,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="B40" t="s">
         <v>24</v>
@@ -949,7 +942,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
         <v>24</v>
@@ -957,7 +950,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
         <v>24</v>
@@ -965,7 +958,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B43" t="s">
         <v>24</v>
@@ -973,23 +966,23 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="B46" t="s">
         <v>24</v>
@@ -997,15 +990,15 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
         <v>24</v>
@@ -1013,7 +1006,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B49" t="s">
         <v>24</v>
@@ -1021,7 +1014,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="B50" t="s">
         <v>24</v>
@@ -1029,7 +1022,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>24</v>
@@ -1037,7 +1030,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
         <v>24</v>
@@ -1045,7 +1038,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
         <v>24</v>
@@ -1053,7 +1046,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
         <v>24</v>
@@ -1061,7 +1054,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
         <v>24</v>
@@ -1069,7 +1062,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
         <v>24</v>
@@ -1077,7 +1070,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
         <v>24</v>
@@ -1085,7 +1078,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
         <v>24</v>
@@ -1093,7 +1086,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B59" t="s">
         <v>24</v>
@@ -1101,7 +1094,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
         <v>24</v>
@@ -1109,7 +1102,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="B61" t="s">
         <v>24</v>
@@ -1117,15 +1110,15 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B63" t="s">
         <v>24</v>
@@ -1133,7 +1126,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B64" t="s">
         <v>24</v>
@@ -1141,23 +1134,23 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B65" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B66" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="B67" t="s">
         <v>24</v>
@@ -1165,7 +1158,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B68" t="s">
         <v>24</v>
@@ -1173,41 +1166,17 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="B69" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B70" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>36</v>
-      </c>
-      <c r="B71" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>65</v>
-      </c>
-      <c r="B72" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>59</v>
-      </c>
-      <c r="B73" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated cure data (v42)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_cure.xlsx
+++ b/src/data/routekaart_status_cure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D7B371-C214-4E10-8796-561644060A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BFD1B3-4ACE-437C-88B4-64642E4E1CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="5250" windowWidth="31400" windowHeight="13130" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="8460" yWindow="1260" windowWidth="26720" windowHeight="19800" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
   <si>
     <t>Amsterdam UMC</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>ZorgSaam Zeeuws-Vlaanderen</t>
+  </si>
+  <si>
+    <t>Roessingh, Centrum voor Revalidatie</t>
   </si>
 </sst>
 </file>
@@ -611,11 +614,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B71"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -977,15 +978,15 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
         <v>24</v>
@@ -993,7 +994,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="B47" t="s">
         <v>24</v>
@@ -1001,7 +1002,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B48" t="s">
         <v>24</v>
@@ -1009,7 +1010,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>24</v>
@@ -1017,7 +1018,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B50" t="s">
         <v>24</v>
@@ -1025,7 +1026,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B51" t="s">
         <v>24</v>
@@ -1033,7 +1034,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
         <v>24</v>
@@ -1041,7 +1042,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B53" t="s">
         <v>24</v>
@@ -1049,7 +1050,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="B54" t="s">
         <v>24</v>
@@ -1057,7 +1058,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B55" t="s">
         <v>24</v>
@@ -1065,7 +1066,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56" t="s">
         <v>24</v>
@@ -1073,7 +1074,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B57" t="s">
         <v>24</v>
@@ -1081,7 +1082,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B58" t="s">
         <v>24</v>
@@ -1089,7 +1090,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="B59" t="s">
         <v>24</v>
@@ -1097,7 +1098,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B60" t="s">
         <v>24</v>
@@ -1105,7 +1106,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
         <v>24</v>
@@ -1113,7 +1114,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B62" t="s">
         <v>24</v>
@@ -1121,7 +1122,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="B63" t="s">
         <v>24</v>
@@ -1129,7 +1130,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B64" t="s">
         <v>24</v>
@@ -1137,7 +1138,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
         <v>24</v>
@@ -1145,23 +1146,23 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B66" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B67" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B68" t="s">
         <v>24</v>
@@ -1169,7 +1170,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B69" t="s">
         <v>24</v>
@@ -1177,7 +1178,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B70" t="s">
         <v>24</v>
@@ -1185,9 +1186,17 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>59</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Udated cure data (v44)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_cure.xlsx
+++ b/src/data/routekaart_status_cure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BFD1B3-4ACE-437C-88B4-64642E4E1CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7937792-D20E-4CE8-8B58-884DF0A07296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="1260" windowWidth="26720" windowHeight="19800" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="18780" yWindow="1050" windowWidth="18850" windowHeight="19120" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="76">
   <si>
     <t>Amsterdam UMC</t>
   </si>
@@ -253,7 +253,10 @@
     <t>ZorgSaam Zeeuws-Vlaanderen</t>
   </si>
   <si>
-    <t>Roessingh, Centrum voor Revalidatie</t>
+    <t>Haaglanden Medisch Centrum</t>
+  </si>
+  <si>
+    <t>Radiotherapiegroep</t>
   </si>
 </sst>
 </file>
@@ -318,9 +321,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -358,7 +361,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -464,7 +467,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -606,7 +609,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -614,7 +617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F40E7E-2647-4F3F-8219-3AF753B4033B}">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -677,7 +680,7 @@
         <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -794,15 +797,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
         <v>24</v>
@@ -810,7 +813,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
@@ -818,7 +821,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
@@ -826,7 +829,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
@@ -834,7 +837,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -842,7 +845,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
         <v>24</v>
@@ -850,7 +853,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
         <v>24</v>
@@ -858,7 +861,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
         <v>24</v>
@@ -866,7 +869,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
@@ -874,7 +877,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
         <v>24</v>
@@ -882,7 +885,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
         <v>24</v>
@@ -890,7 +893,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
         <v>24</v>
@@ -898,7 +901,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
         <v>24</v>
@@ -906,7 +909,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
         <v>24</v>
@@ -914,7 +917,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
         <v>24</v>
@@ -922,7 +925,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
         <v>24</v>
@@ -930,7 +933,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
         <v>24</v>
@@ -938,7 +941,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
         <v>24</v>
@@ -946,7 +949,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B41" t="s">
         <v>24</v>
@@ -954,7 +957,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
         <v>24</v>
@@ -962,7 +965,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="B43" t="s">
         <v>24</v>
@@ -970,7 +973,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
         <v>23</v>
@@ -978,23 +981,23 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
         <v>24</v>
@@ -1002,7 +1005,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="B48" t="s">
         <v>24</v>
@@ -1010,7 +1013,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
         <v>24</v>
@@ -1018,7 +1021,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>24</v>
@@ -1026,7 +1029,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B51" t="s">
         <v>24</v>
@@ -1034,7 +1037,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
         <v>24</v>
@@ -1042,7 +1045,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
         <v>24</v>
@@ -1050,7 +1053,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B54" t="s">
         <v>24</v>
@@ -1058,7 +1061,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="B55" t="s">
         <v>24</v>
@@ -1066,7 +1069,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B56" t="s">
         <v>24</v>
@@ -1074,7 +1077,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57" t="s">
         <v>24</v>
@@ -1082,7 +1085,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58" t="s">
         <v>24</v>
@@ -1090,7 +1093,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B59" t="s">
         <v>24</v>
@@ -1098,7 +1101,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
         <v>24</v>
@@ -1106,7 +1109,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B61" t="s">
         <v>24</v>
@@ -1114,7 +1117,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
         <v>24</v>
@@ -1122,7 +1125,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B63" t="s">
         <v>24</v>
@@ -1130,7 +1133,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="B64" t="s">
         <v>24</v>
@@ -1138,7 +1141,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B65" t="s">
         <v>24</v>
@@ -1146,7 +1149,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="B66" t="s">
         <v>24</v>
@@ -1154,23 +1157,23 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B67" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B69" t="s">
         <v>24</v>
@@ -1178,7 +1181,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B70" t="s">
         <v>24</v>
@@ -1186,7 +1189,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B71" t="s">
         <v>24</v>
@@ -1194,9 +1197,17 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>59</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated cure data (v45)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_cure.xlsx
+++ b/src/data/routekaart_status_cure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7937792-D20E-4CE8-8B58-884DF0A07296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E25CDAB-41DF-49BD-9C62-5D8107887786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18780" yWindow="1050" windowWidth="18850" windowHeight="19120" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="7550" yWindow="2230" windowWidth="28800" windowHeight="15370" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -800,7 +800,7 @@
         <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated cure data (v46)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_cure.xlsx
+++ b/src/data/routekaart_status_cure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E25CDAB-41DF-49BD-9C62-5D8107887786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3D2053-7697-41C1-8689-2AB6649CFAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7550" yWindow="2230" windowWidth="28800" windowHeight="15370" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="3600" yWindow="750" windowWidth="33345" windowHeight="19410" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -621,13 +621,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.7265625" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
@@ -635,7 +635,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -643,7 +643,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -651,15 +651,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -667,7 +667,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -675,7 +675,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -683,7 +683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -691,7 +691,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -699,7 +699,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -707,7 +707,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -715,7 +715,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -723,7 +723,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -731,7 +731,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -739,7 +739,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -747,7 +747,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -755,7 +755,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -763,7 +763,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -771,7 +771,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -779,7 +779,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -787,7 +787,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -795,7 +795,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -803,7 +803,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -811,7 +811,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -819,7 +819,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -827,7 +827,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -835,7 +835,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -843,7 +843,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -851,7 +851,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -859,7 +859,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -867,7 +867,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -875,7 +875,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -883,7 +883,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -891,7 +891,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -899,7 +899,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -907,7 +907,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -915,7 +915,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -923,7 +923,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -931,7 +931,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -939,7 +939,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -947,7 +947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -955,7 +955,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>61</v>
       </c>
@@ -963,7 +963,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -971,7 +971,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>75</v>
       </c>
@@ -979,7 +979,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -987,7 +987,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -995,7 +995,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>34</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>19</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>51</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>52</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>53</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>54</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>55</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>64</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>56</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>22</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>58</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>35</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>20</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>21</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>36</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>65</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
Updated data for cure (v47; Frisius MC)
</commit_message>
<xml_diff>
--- a/src/data/routekaart_status_cure.xlsx
+++ b/src/data/routekaart_status_cure.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3D2053-7697-41C1-8689-2AB6649CFAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF744C0A-D195-4964-9221-4ED8670C9A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="750" windowWidth="33345" windowHeight="19410" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
+    <workbookView xWindow="5895" yWindow="2610" windowWidth="31590" windowHeight="17385" xr2:uid="{8CE8C91A-5D2B-429A-9150-16FF2E6CA716}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,9 +169,6 @@
     <t>LUMC</t>
   </si>
   <si>
-    <t>Medisch Centrum Leeuwarden</t>
-  </si>
-  <si>
     <t>Prinses Máxima Centrum</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
     <t>Stichting Ziekenhuisgroep Twente (ZGT)</t>
   </si>
   <si>
-    <t>Tjongerschans</t>
-  </si>
-  <si>
     <t>UMC Utrecht</t>
   </si>
   <si>
@@ -257,6 +251,12 @@
   </si>
   <si>
     <t>Radiotherapiegroep</t>
+  </si>
+  <si>
+    <t>Frisius MC locatie Leeuwarden</t>
+  </si>
+  <si>
+    <t>Frisius MC locatie Heerenveen</t>
   </si>
 </sst>
 </file>
@@ -629,7 +629,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>25</v>
@@ -637,7 +637,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
         <v>24</v>
@@ -837,7 +837,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
         <v>24</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
         <v>24</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B41" t="s">
         <v>24</v>
@@ -957,7 +957,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B42" t="s">
         <v>24</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43" t="s">
         <v>24</v>
@@ -973,7 +973,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B44" t="s">
         <v>23</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
         <v>24</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B47" t="s">
         <v>24</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B49" t="s">
         <v>24</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
         <v>24</v>
@@ -1045,7 +1045,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B53" t="s">
         <v>24</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B56" t="s">
         <v>24</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B57" t="s">
         <v>24</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B58" t="s">
         <v>24</v>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B59" t="s">
         <v>24</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B61" t="s">
         <v>24</v>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
         <v>24</v>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B63" t="s">
         <v>24</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
         <v>24</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B66" t="s">
         <v>24</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B71" t="s">
         <v>24</v>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>24</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B73" t="s">
         <v>24</v>

</xml_diff>